<commit_message>
Fixed QB/DST, add autofull, change theme and layout
</commit_message>
<xml_diff>
--- a/data/FormatedDSTProjections.xlsx
+++ b/data/FormatedDSTProjections.xlsx
@@ -5,28 +5,28 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethankatnic/Desktop/FantasyProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethankatnic/Desktop/FantasyProject/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="460" windowWidth="25360" windowHeight="15540" firstSheet="4" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2 (16)" sheetId="18" r:id="rId1"/>
-    <sheet name="Sheet2 (15)" sheetId="17" r:id="rId2"/>
-    <sheet name="Sheet2 (14)" sheetId="16" r:id="rId3"/>
-    <sheet name="Sheet2 (13)" sheetId="15" r:id="rId4"/>
-    <sheet name="Sheet2 (12)" sheetId="14" r:id="rId5"/>
-    <sheet name="Sheet2 (11)" sheetId="13" r:id="rId6"/>
-    <sheet name="Sheet2 (10)" sheetId="12" r:id="rId7"/>
-    <sheet name="Sheet2 (9)" sheetId="11" r:id="rId8"/>
-    <sheet name="Sheet2 (8)" sheetId="10" r:id="rId9"/>
-    <sheet name="Sheet2 (7)" sheetId="9" r:id="rId10"/>
-    <sheet name="Sheet2 (6)" sheetId="8" r:id="rId11"/>
-    <sheet name="Sheet2 (5)" sheetId="7" r:id="rId12"/>
-    <sheet name="Sheet2 (4)" sheetId="6" r:id="rId13"/>
-    <sheet name="Sheet2 (3)" sheetId="5" r:id="rId14"/>
-    <sheet name="Sheet2 (2)" sheetId="4" r:id="rId15"/>
+    <sheet name="Sheet2 (16)" sheetId="33" r:id="rId1"/>
+    <sheet name="Sheet2 (15)" sheetId="32" r:id="rId2"/>
+    <sheet name="Sheet2 (14)" sheetId="31" r:id="rId3"/>
+    <sheet name="Sheet2 (13)" sheetId="30" r:id="rId4"/>
+    <sheet name="Sheet2 (12)" sheetId="29" r:id="rId5"/>
+    <sheet name="Sheet2 (11)" sheetId="28" r:id="rId6"/>
+    <sheet name="Sheet2 (10)" sheetId="27" r:id="rId7"/>
+    <sheet name="Sheet2 (9)" sheetId="26" r:id="rId8"/>
+    <sheet name="Sheet2 (8)" sheetId="25" r:id="rId9"/>
+    <sheet name="Sheet2 (7)" sheetId="24" r:id="rId10"/>
+    <sheet name="Sheet2 (6)" sheetId="23" r:id="rId11"/>
+    <sheet name="Sheet2 (5)" sheetId="22" r:id="rId12"/>
+    <sheet name="Sheet2 (4)" sheetId="21" r:id="rId13"/>
+    <sheet name="Sheet2 (3)" sheetId="20" r:id="rId14"/>
+    <sheet name="Sheet2 (2)" sheetId="19" r:id="rId15"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId16"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -51,9 +51,6 @@
     <t>Minnesota Min - DEF</t>
   </si>
   <si>
-    <t>Los Angeles LAR - DEF</t>
-  </si>
-  <si>
     <t>Denver Den - DEF</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
   </si>
   <si>
     <t>Tennessee Ten - DEF</t>
-  </si>
-  <si>
-    <t>Los Angeles LAC - DEF</t>
   </si>
   <si>
     <t>Chicago Chi - DEF</t>
@@ -115,6 +109,12 @@
   </si>
   <si>
     <t>Tampa Bay TB - DEF</t>
+  </si>
+  <si>
+    <t>Los Angeles Rams LAR - DEF</t>
+  </si>
+  <si>
+    <t>Los Angeles Chargers LAC - DEF</t>
   </si>
 </sst>
 </file>
@@ -557,16 +557,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC42AEF-68EA-BE4B-BEA4-6CBE7A21253C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD963991-8743-2541-8D14-11A71794282B}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -604,7 +604,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -612,7 +612,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -668,7 +668,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -716,7 +716,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -732,7 +732,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -784,16 +784,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D67E53A-A341-BF4B-98C7-A35894123F8E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E993ED37-A16D-0444-A540-9CAB0F11A0C0}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -831,7 +831,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -863,7 +863,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -895,7 +895,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -903,7 +903,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -919,7 +919,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -943,7 +943,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -951,7 +951,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -959,7 +959,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -975,7 +975,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -983,7 +983,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -1011,16 +1011,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB021CD-26CD-424A-B274-872D7F493D3E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5A2F84-83DB-0546-8F8F-46B1BD8FA789}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -1122,7 +1122,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -1138,7 +1138,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -1146,7 +1146,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -1178,7 +1178,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -1194,7 +1194,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -1202,7 +1202,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -1210,7 +1210,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -1218,7 +1218,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -1238,16 +1238,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F7BC17-340F-534E-8536-9554809500DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A1B13C1-7959-F348-859A-27A943AAAF62}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1285,7 +1285,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -1301,7 +1301,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -1309,7 +1309,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -1317,7 +1317,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -1325,7 +1325,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -1333,7 +1333,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -1341,7 +1341,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -1349,7 +1349,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -1365,7 +1365,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -1373,7 +1373,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -1389,7 +1389,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -1405,7 +1405,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -1437,7 +1437,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -1465,16 +1465,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394F10F7-A82C-044E-9B2C-5418FE8D31C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE1C13E-3AD3-1943-9D0D-5D10D4CD577E}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1512,7 +1512,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -1528,7 +1528,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -1656,7 +1656,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -1672,7 +1672,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -1692,16 +1692,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472CBD19-1FD5-A349-B45D-99E7830252C0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B007A7-A206-6044-A7EF-FC7EBA699C34}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -1763,7 +1763,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -1779,7 +1779,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -1819,7 +1819,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -1859,7 +1859,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -1883,7 +1883,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -1919,16 +1919,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9DE981B-B4DD-8644-B88C-435E9E4DA9EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ECE5AE-1FE7-594F-AC83-2E62568070D2}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -1982,7 +1982,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -1990,7 +1990,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -2006,7 +2006,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -2014,7 +2014,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -2054,7 +2054,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -2086,7 +2086,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -2094,7 +2094,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -2102,7 +2102,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -2118,7 +2118,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -2149,13 +2149,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2193,7 +2193,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -2201,7 +2201,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -2217,7 +2217,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -2225,7 +2225,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -2233,7 +2233,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -2241,7 +2241,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -2249,7 +2249,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -2265,7 +2265,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -2281,7 +2281,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -2289,7 +2289,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -2305,7 +2305,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -2313,7 +2313,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -2321,7 +2321,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -2329,7 +2329,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -2337,7 +2337,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -2353,7 +2353,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -2361,7 +2361,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -2373,16 +2373,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E473408F-120D-BA4E-8F52-5F62B77A7E6A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194C03F2-343C-D04E-8144-DAF7884935A5}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -2436,7 +2436,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -2452,7 +2452,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -2460,7 +2460,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -2468,7 +2468,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -2476,7 +2476,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -2492,7 +2492,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -2500,7 +2500,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -2508,7 +2508,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -2532,7 +2532,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -2540,7 +2540,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -2548,7 +2548,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -2556,7 +2556,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -2572,7 +2572,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -2588,7 +2588,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -2600,16 +2600,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DD3343-98BC-CC4C-B2FD-4D5210152704}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E78A6F6-5212-B84A-BD9C-A8F2584BF0BB}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -2663,7 +2663,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -2695,7 +2695,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -2703,7 +2703,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -2711,7 +2711,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -2719,7 +2719,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -2727,7 +2727,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -2743,7 +2743,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -2759,7 +2759,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -2767,7 +2767,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -2775,7 +2775,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -2783,7 +2783,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -2799,7 +2799,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -2807,7 +2807,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -2815,7 +2815,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -2827,16 +2827,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{167474CD-A88C-8E49-813A-CF12E4433C7D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8382B634-420E-BE4D-91DA-2D8CA69C1992}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2874,7 +2874,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -2882,7 +2882,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -2890,7 +2890,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -2898,7 +2898,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -2906,7 +2906,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -2914,7 +2914,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -2930,7 +2930,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -2938,7 +2938,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -2946,7 +2946,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -2962,7 +2962,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -2970,7 +2970,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -2986,7 +2986,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -3002,7 +3002,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -3018,7 +3018,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -3034,7 +3034,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -3042,7 +3042,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -3054,16 +3054,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B7A7AA-1A6C-4B41-B9C8-79C19B943CF0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECF9C41-67ED-8642-9032-9101068D5975}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3101,7 +3101,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -3109,7 +3109,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -3117,7 +3117,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -3125,7 +3125,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -3133,7 +3133,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -3149,7 +3149,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -3157,7 +3157,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -3165,7 +3165,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -3173,7 +3173,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -3189,7 +3189,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -3197,7 +3197,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -3205,7 +3205,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -3213,7 +3213,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -3221,7 +3221,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -3229,7 +3229,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -3237,7 +3237,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -3245,7 +3245,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -3253,7 +3253,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -3261,7 +3261,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -3269,7 +3269,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -3281,16 +3281,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44708001-F1CE-2D4C-8B9A-3DFF7819B941}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB320067-3A0B-C54C-A7E8-E55C41C241D2}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3328,7 +3328,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -3336,7 +3336,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -3344,7 +3344,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -3352,7 +3352,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -3360,7 +3360,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -3368,7 +3368,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -3376,7 +3376,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -3384,7 +3384,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -3392,7 +3392,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -3400,7 +3400,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -3408,7 +3408,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -3416,7 +3416,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -3424,7 +3424,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -3432,7 +3432,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -3440,7 +3440,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -3448,7 +3448,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -3456,7 +3456,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -3472,7 +3472,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -3480,7 +3480,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -3488,7 +3488,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -3496,7 +3496,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -3508,16 +3508,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEE2AEF-BBCB-7941-89CE-8DF1F3F59113}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{992EC443-A384-364C-81FA-B5AF5771B910}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3555,7 +3555,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -3563,7 +3563,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -3571,7 +3571,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -3579,7 +3579,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -3587,7 +3587,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -3595,7 +3595,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -3603,7 +3603,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -3611,7 +3611,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -3619,7 +3619,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -3627,7 +3627,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -3635,7 +3635,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -3643,7 +3643,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -3651,7 +3651,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -3659,7 +3659,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -3667,7 +3667,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -3675,7 +3675,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -3691,7 +3691,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -3699,7 +3699,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -3707,7 +3707,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -3715,7 +3715,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -3723,7 +3723,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -3735,16 +3735,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8561361-2DA1-1946-A8EB-211C3DFCDFB4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2180750B-F104-D246-BE91-68A49914C9F5}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3782,7 +3782,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -3790,7 +3790,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -3798,7 +3798,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -3806,7 +3806,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -3814,7 +3814,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -3822,7 +3822,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -3830,7 +3830,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -3838,7 +3838,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -3846,7 +3846,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -3854,7 +3854,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -3862,7 +3862,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -3870,7 +3870,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -3878,7 +3878,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -3886,7 +3886,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -3894,7 +3894,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -3902,7 +3902,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -3910,7 +3910,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -3918,7 +3918,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -3926,7 +3926,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -3942,7 +3942,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -3950,7 +3950,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>
@@ -3962,16 +3962,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A6AF47-D521-A54E-B495-30A3F7472419}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9DD040F-D19F-2B48-AF6B-8880633EB1D9}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4009,7 +4009,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>7.9587500000000002</v>
@@ -4017,7 +4017,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>7.9225000000000003</v>
@@ -4025,7 +4025,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>7.4187500000000002</v>
@@ -4033,7 +4033,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>6.6837499999999999</v>
@@ -4041,7 +4041,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>6.586875</v>
@@ -4049,7 +4049,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>6.5706249999999997</v>
@@ -4057,7 +4057,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>6.4993749999999997</v>
@@ -4065,7 +4065,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>6.4762500000000003</v>
@@ -4073,7 +4073,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>6.3787500000000001</v>
@@ -4081,7 +4081,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>6.24125</v>
@@ -4089,7 +4089,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>6.194375</v>
@@ -4097,7 +4097,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>6.131875</v>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>6.0856250000000003</v>
@@ -4113,7 +4113,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
         <v>5.9743750000000002</v>
@@ -4121,7 +4121,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4">
         <v>5.9187500000000002</v>
@@ -4129,7 +4129,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4">
         <v>5.8825000000000003</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4">
         <v>5.78</v>
@@ -4145,7 +4145,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
         <v>5.71875</v>
@@ -4153,7 +4153,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5.6687500000000002</v>
@@ -4161,7 +4161,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4">
         <v>5.5862499999999997</v>
@@ -4169,7 +4169,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="4">
         <v>5.3137499999999998</v>
@@ -4177,7 +4177,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>5.2718749999999996</v>

</xml_diff>